<commit_message>
se actuliza el arbol de kruskal y las imagenes del MDI con su codigo
</commit_message>
<xml_diff>
--- a/Fundamentos de la ingenieria/Burndown Chart del Sprint1.xlsx
+++ b/Fundamentos de la ingenieria/Burndown Chart del Sprint1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhon fonseca\Documents\Proyecto del clase\Fundamentos de la ingenieria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1BD8636-E8F0-45B5-9883-32B67A6FCD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5888355B-E0CB-47F0-A246-FFE6F6BDA8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B08D63F-2712-47D5-9BB1-3EF66162EFC9}"/>
   </bookViews>
@@ -331,7 +331,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
@@ -707,7 +707,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
@@ -933,6 +933,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="553903024"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1903,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990EDF44-9C51-4955-9882-42B0DB4A1CAE}">
   <dimension ref="A2:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2">
         <v>7</v>
@@ -2039,7 +2040,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
         <v>7</v>

</xml_diff>